<commit_message>
added delete functionality in dataframe.py file
</commit_message>
<xml_diff>
--- a/multi/repo/repo.xlsx
+++ b/multi/repo/repo.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -486,12 +486,12 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>eae00c4f-c06c-47e5-862c-32e2a05dd8c2</t>
+          <t>055354a9-ebaf-41ca-904b-d346b8abbac4</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>data11 - Copy.xlsx</t>
+          <t>data11.xlsx</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -501,7 +501,7 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>2024-08-13 18:22:34</t>
+          <t>2024-08-13 19:12:01</t>
         </is>
       </c>
       <c r="E3" t="inlineStr"/>
@@ -509,7 +509,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>055354a9-ebaf-41ca-904b-d346b8abbac4</t>
+          <t>b84f2133-a825-4c23-aed9-750c96634fed</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -524,7 +524,7 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>2024-08-13 19:12:01</t>
+          <t>2024-08-13 20:15:13</t>
         </is>
       </c>
       <c r="E4" t="inlineStr"/>
@@ -532,7 +532,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>b84f2133-a825-4c23-aed9-750c96634fed</t>
+          <t>a58c6fb5-2767-4a4f-ad86-68ffa5fcefa2</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -547,7 +547,7 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>2024-08-13 20:15:13</t>
+          <t>2024-08-14 09:59:40</t>
         </is>
       </c>
       <c r="E5" t="inlineStr"/>
@@ -555,7 +555,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>a58c6fb5-2767-4a4f-ad86-68ffa5fcefa2</t>
+          <t>015922ea-0b89-4d26-9bda-992a1e553322</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -570,7 +570,7 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>2024-08-14 09:59:40</t>
+          <t>2024-08-14 10:00:56</t>
         </is>
       </c>
       <c r="E6" t="inlineStr"/>
@@ -578,12 +578,12 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>89597334-4aa6-4dcc-8b9c-16ddfa4b9178</t>
+          <t>5a0a3cdd-0e08-4ec1-a6f0-71a7856a120e</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>data11 - Copy.xlsx</t>
+          <t>data11.xlsx</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -593,125 +593,10 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>2024-08-14 09:59:55</t>
+          <t>2024-08-14 11:07:13</t>
         </is>
       </c>
       <c r="E7" t="inlineStr"/>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>015922ea-0b89-4d26-9bda-992a1e553322</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>data11.xlsx</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>initiated</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>2024-08-14 10:00:56</t>
-        </is>
-      </c>
-      <c r="E8" t="inlineStr"/>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>5a0a3cdd-0e08-4ec1-a6f0-71a7856a120e</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>data11.xlsx</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>initiated</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>2024-08-14 11:07:13</t>
-        </is>
-      </c>
-      <c r="E9" t="inlineStr"/>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>8fdc9d60-a2cc-4546-abe4-bc966a06c955</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>data11 - Copy.xlsx</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>initiated</t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>2024-08-14 11:07:32</t>
-        </is>
-      </c>
-      <c r="E10" t="inlineStr"/>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>d465c3ad-fc6a-47b9-bc4e-9cea8a539a55</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>data13.xlsx</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>initiated</t>
-        </is>
-      </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>2024-08-19 16:23:38</t>
-        </is>
-      </c>
-      <c r="E11" t="inlineStr"/>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>65bddbed-6f23-4dd7-9e20-83334477b778</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>data14.xlsx</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>initiated</t>
-        </is>
-      </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>2024-08-19 16:23:58</t>
-        </is>
-      </c>
-      <c r="E12" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
two folders and 2 pages structure
</commit_message>
<xml_diff>
--- a/multi/repo/repo.xlsx
+++ b/multi/repo/repo.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -598,6 +598,79 @@
       </c>
       <c r="E7" t="inlineStr"/>
     </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>a490a4ea-2d1f-4201-9005-2115f8439b35</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>data14.xlsx</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>initiated</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>2024-08-21 15:40:10</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr"/>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>71c964c7-6668-4b41-8201-89524dc87d0b</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>data13.xlsx</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>initiated</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>2024-08-22 12:04:18</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr"/>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>2a5fea97-05a6-42f8-bbcc-37ad2fa849a9</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>data13.xlsx</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>initiated</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>2024-08-22 13:41:55</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>